<commit_message>
update TR and ATR tests
</commit_message>
<xml_diff>
--- a/tests/indicators/s-z/Tr/Tr.Calc.xlsx
+++ b/tests/indicators/s-z/Tr/Tr.Calc.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BDF24A1-02C3-4770-9108-9C14E8020AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C874ED7-951C-44F0-848B-3A549CC04043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3690" yWindow="1140" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TR" sheetId="1" r:id="rId1"/>
@@ -575,7 +575,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1335,22 +1335,14 @@
       <c r="G2" s="1">
         <v>96708880</v>
       </c>
-      <c r="H2" s="2">
-        <f>testdata[[#This Row],[high]]-testdata[[#This Row],[low]]</f>
-        <v>1.8299999999999841</v>
-      </c>
+      <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
-      <c r="K2" s="9">
-        <f>MAX(testdata[[#This Row],[H-L]:[|L-pC|]])</f>
-        <v>1.8299999999999841</v>
-      </c>
+      <c r="K2" s="11"/>
       <c r="M2" s="3">
         <v>42738</v>
       </c>
-      <c r="N2" s="9">
-        <v>1.83</v>
-      </c>
+      <c r="N2" s="11"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
@@ -1386,14 +1378,14 @@
         <f>ABS(testdata[[#This Row],[low]]-F2)</f>
         <v>0.34999999999999432</v>
       </c>
-      <c r="K3" s="9">
+      <c r="K3" s="11">
         <f>MAX(testdata[[#This Row],[H-L]:[|L-pC|]])</f>
         <v>1.4199999999999875</v>
       </c>
       <c r="M3" s="3">
         <v>42739</v>
       </c>
-      <c r="N3" s="9">
+      <c r="N3" s="11">
         <v>1.42</v>
       </c>
     </row>
@@ -1881,14 +1873,14 @@
         <f>ABS(testdata[[#This Row],[low]]-F13)</f>
         <v>6.0000000000002274E-2</v>
       </c>
-      <c r="K14" s="9">
+      <c r="K14" s="11">
         <f>MAX(testdata[[#This Row],[H-L]:[|L-pC|]])</f>
         <v>1.3199999999999932</v>
       </c>
       <c r="M14" s="3">
         <v>42755</v>
       </c>
-      <c r="N14" s="9">
+      <c r="N14" s="11">
         <v>1.32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update TR initialization (#949)
* update TR and ATR
* adjust ADX
* adjust ATR Stop
* adjust Chandelier Exit
* adjust STARC Bands
* adjust SuperTrend
* adjust  Volatility Stop
</commit_message>
<xml_diff>
--- a/tests/indicators/s-z/Tr/Tr.Calc.xlsx
+++ b/tests/indicators/s-z/Tr/Tr.Calc.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BDF24A1-02C3-4770-9108-9C14E8020AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C874ED7-951C-44F0-848B-3A549CC04043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3690" yWindow="1140" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TR" sheetId="1" r:id="rId1"/>
@@ -575,7 +575,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1335,22 +1335,14 @@
       <c r="G2" s="1">
         <v>96708880</v>
       </c>
-      <c r="H2" s="2">
-        <f>testdata[[#This Row],[high]]-testdata[[#This Row],[low]]</f>
-        <v>1.8299999999999841</v>
-      </c>
+      <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
-      <c r="K2" s="9">
-        <f>MAX(testdata[[#This Row],[H-L]:[|L-pC|]])</f>
-        <v>1.8299999999999841</v>
-      </c>
+      <c r="K2" s="11"/>
       <c r="M2" s="3">
         <v>42738</v>
       </c>
-      <c r="N2" s="9">
-        <v>1.83</v>
-      </c>
+      <c r="N2" s="11"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
@@ -1386,14 +1378,14 @@
         <f>ABS(testdata[[#This Row],[low]]-F2)</f>
         <v>0.34999999999999432</v>
       </c>
-      <c r="K3" s="9">
+      <c r="K3" s="11">
         <f>MAX(testdata[[#This Row],[H-L]:[|L-pC|]])</f>
         <v>1.4199999999999875</v>
       </c>
       <c r="M3" s="3">
         <v>42739</v>
       </c>
-      <c r="N3" s="9">
+      <c r="N3" s="11">
         <v>1.42</v>
       </c>
     </row>
@@ -1881,14 +1873,14 @@
         <f>ABS(testdata[[#This Row],[low]]-F13)</f>
         <v>6.0000000000002274E-2</v>
       </c>
-      <c r="K14" s="9">
+      <c r="K14" s="11">
         <f>MAX(testdata[[#This Row],[H-L]:[|L-pC|]])</f>
         <v>1.3199999999999932</v>
       </c>
       <c r="M14" s="3">
         <v>42755</v>
       </c>
-      <c r="N14" s="9">
+      <c r="N14" s="11">
         <v>1.32</v>
       </c>
     </row>

</xml_diff>